<commit_message>
description.en an gra2005 angepasst
</commit_message>
<xml_diff>
--- a/data/instruments/instruments.xlsx
+++ b/data/instruments/instruments.xlsx
@@ -11,7 +11,7 @@
     <sheet name="attachments" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -195,9 +195,6 @@
     <t>visualization of the survey procedures controlled by filter questions</t>
   </si>
   <si>
-    <t>mapping of questions of the survey instrument and variables of the data set</t>
-  </si>
-  <si>
     <t>Fragebogen des Studienberechtigtenpanels 2008 - zweite Welle</t>
   </si>
   <si>
@@ -241,13 +238,16 @@
   </si>
   <si>
     <t>Questionnaire of third wave of German School Leavers Survey 2008</t>
+  </si>
+  <si>
+    <t>mapping between questions of the survey instrument and variables of the data set</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -267,6 +267,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -289,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -318,6 +325,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -670,16 +683,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
@@ -693,16 +706,16 @@
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E3" t="s">
         <v>55</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G3" t="s">
         <v>7</v>
@@ -716,16 +729,16 @@
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E4" t="s">
         <v>56</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G4" t="s">
         <v>7</v>
@@ -749,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,7 +795,7 @@
       <c r="E1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="17" t="s">
         <v>16</v>
       </c>
       <c r="G1" s="4" t="s">
@@ -809,7 +822,7 @@
       <c r="E2" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="17" t="s">
         <v>57</v>
       </c>
       <c r="G2" t="s">
@@ -835,7 +848,7 @@
       <c r="E3" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="17" t="s">
         <v>58</v>
       </c>
       <c r="G3" t="s">
@@ -861,8 +874,8 @@
       <c r="E4" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="15" t="s">
-        <v>59</v>
+      <c r="F4" s="16" t="s">
+        <v>74</v>
       </c>
       <c r="G4" t="s">
         <v>20</v>
@@ -887,7 +900,7 @@
       <c r="E5" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="17" t="s">
         <v>57</v>
       </c>
       <c r="G5" t="s">
@@ -913,7 +926,7 @@
       <c r="E6" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="17" t="s">
         <v>58</v>
       </c>
       <c r="G6" t="s">
@@ -939,8 +952,8 @@
       <c r="E7" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="F7" s="15" t="s">
-        <v>59</v>
+      <c r="F7" s="16" t="s">
+        <v>74</v>
       </c>
       <c r="G7" t="s">
         <v>20</v>
@@ -965,7 +978,7 @@
       <c r="E8" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="17" t="s">
         <v>57</v>
       </c>
       <c r="G8" t="s">
@@ -991,7 +1004,7 @@
       <c r="E9" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="17" t="s">
         <v>58</v>
       </c>
       <c r="G9" t="s">
@@ -1017,8 +1030,8 @@
       <c r="E10" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="15" t="s">
-        <v>59</v>
+      <c r="F10" s="16" t="s">
+        <v>74</v>
       </c>
       <c r="G10" t="s">
         <v>20</v>
@@ -1144,7 +1157,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>23</v>
@@ -1167,7 +1180,7 @@
     </row>
     <row r="17" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>23</v>
@@ -1191,7 +1204,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>23</v>
@@ -1262,7 +1275,7 @@
     </row>
     <row r="21" spans="1:9" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>23</v>
@@ -1286,7 +1299,7 @@
     </row>
     <row r="22" spans="1:9" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>23</v>
@@ -1310,7 +1323,7 @@
     </row>
     <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>23</v>
@@ -1333,7 +1346,7 @@
     </row>
     <row r="24" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>23</v>
@@ -1357,7 +1370,7 @@
     </row>
     <row r="25" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>23</v>
@@ -1381,7 +1394,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>23</v>
@@ -1404,7 +1417,7 @@
     </row>
     <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>23</v>
@@ -1427,7 +1440,7 @@
     </row>
     <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>23</v>
@@ -1450,7 +1463,7 @@
     </row>
     <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>23</v>
@@ -1473,7 +1486,7 @@
     </row>
     <row r="30" spans="1:9" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B30" s="10" t="s">
         <v>23</v>
@@ -1497,7 +1510,7 @@
     </row>
     <row r="31" spans="1:9" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B31" s="10" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Reihenfolge attachments, engl. Ü.
</commit_message>
<xml_diff>
--- a/data/instruments/instruments.xlsx
+++ b/data/instruments/instruments.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14385" yWindow="-15" windowWidth="14430" windowHeight="14550" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="14385" yWindow="-15" windowWidth="14430" windowHeight="14550" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="instruments" sheetId="1" r:id="rId1"/>
     <sheet name="attachments" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -195,15 +195,6 @@
     <t>visualization of the survey procedures controlled by filter questions</t>
   </si>
   <si>
-    <t>Fragebogen des Studienberechtigtenpanels 2008 - zweite Welle</t>
-  </si>
-  <si>
-    <t>Fragebogen des Studienberechtigtenpanels 2008 - erste Welle</t>
-  </si>
-  <si>
-    <t>Fragebogen des Studienberechtigtenpanels 2008 - dritte Welle</t>
-  </si>
-  <si>
     <t>cl-dzhw-6.xlsx</t>
   </si>
   <si>
@@ -231,29 +222,45 @@
     <t>Education, career and life paths</t>
   </si>
   <si>
-    <t>Questionnaire of first wave of German School Leavers Survey 2008</t>
-  </si>
-  <si>
-    <t>Questionnaire of second wave of German School Leavers Survey 2008</t>
-  </si>
-  <si>
-    <t>Questionnaire of third wave of German School Leavers Survey 2008</t>
-  </si>
-  <si>
     <t>mapping between questions of the survey instrument and variables of the data set</t>
+  </si>
+  <si>
+    <t>Fragebogen des DZHW-Studienberechtigtenpanels 2008 - erste Welle</t>
+  </si>
+  <si>
+    <t>Fragebogen des DZHW-Studienberechtigtenpanels 2008 - zweite Welle</t>
+  </si>
+  <si>
+    <t>Fragebogen des DZHW-Studienberechtigtenpanels 2008 - dritte Welle</t>
+  </si>
+  <si>
+    <t>Questionnaire of the DZHW Panel Study of School Leavers 2008 - first wave</t>
+  </si>
+  <si>
+    <t>Questionnaire of the DZHW Panel Study of School Leavers 2008 - second wave</t>
+  </si>
+  <si>
+    <t>Questionnaire of the DZHW Panel Study of School Leavers 2008 - third wave</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -275,6 +282,13 @@
       <charset val="1"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -293,13 +307,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -314,28 +330,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard 2" xfId="2"/>
+    <cellStyle name="Standard 3" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -636,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,16 +674,16 @@
       <c r="B1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" t="s">
         <v>16</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
       <c r="G1" t="s">
@@ -682,17 +697,17 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>71</v>
+      <c r="C2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" t="s">
+        <v>72</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>68</v>
+      <c r="F2" t="s">
+        <v>65</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
@@ -705,17 +720,17 @@
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>72</v>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
+        <v>73</v>
       </c>
       <c r="E3" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="14" t="s">
-        <v>69</v>
+      <c r="F3" t="s">
+        <v>66</v>
       </c>
       <c r="G3" t="s">
         <v>7</v>
@@ -728,17 +743,17 @@
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>73</v>
+      <c r="C4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" t="s">
+        <v>74</v>
       </c>
       <c r="E4" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>70</v>
+      <c r="F4" t="s">
+        <v>67</v>
       </c>
       <c r="G4" t="s">
         <v>7</v>
@@ -760,10 +775,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,7 +788,7 @@
     <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="51.28515625" style="5" customWidth="1"/>
     <col min="5" max="5" width="62.42578125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="46.42578125" style="15" customWidth="1"/>
+    <col min="6" max="6" width="46.42578125" style="14" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" customWidth="1"/>
     <col min="8" max="8" width="18" style="1" customWidth="1"/>
     <col min="9" max="1027" width="10.5703125"/>
@@ -795,7 +810,7 @@
       <c r="E1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>16</v>
       </c>
       <c r="G1" s="4" t="s">
@@ -822,7 +837,7 @@
       <c r="E2" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="16" t="s">
         <v>57</v>
       </c>
       <c r="G2" t="s">
@@ -848,7 +863,7 @@
       <c r="E3" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="16" t="s">
         <v>58</v>
       </c>
       <c r="G3" t="s">
@@ -874,8 +889,8 @@
       <c r="E4" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="16" t="s">
-        <v>74</v>
+      <c r="F4" s="15" t="s">
+        <v>68</v>
       </c>
       <c r="G4" t="s">
         <v>20</v>
@@ -900,7 +915,7 @@
       <c r="E5" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="16" t="s">
         <v>57</v>
       </c>
       <c r="G5" t="s">
@@ -926,7 +941,7 @@
       <c r="E6" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="16" t="s">
         <v>58</v>
       </c>
       <c r="G6" t="s">
@@ -952,8 +967,8 @@
       <c r="E7" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="F7" s="16" t="s">
-        <v>74</v>
+      <c r="F7" s="15" t="s">
+        <v>68</v>
       </c>
       <c r="G7" t="s">
         <v>20</v>
@@ -978,7 +993,7 @@
       <c r="E8" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="16" t="s">
         <v>57</v>
       </c>
       <c r="G8" t="s">
@@ -1004,7 +1019,7 @@
       <c r="E9" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="16" t="s">
         <v>58</v>
       </c>
       <c r="G9" t="s">
@@ -1030,8 +1045,8 @@
       <c r="E10" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="16" t="s">
-        <v>74</v>
+      <c r="F10" s="15" t="s">
+        <v>68</v>
       </c>
       <c r="G10" t="s">
         <v>20</v>
@@ -1040,55 +1055,56 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>20</v>
       </c>
       <c r="H11" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="12" t="s">
         <v>24</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="1">
-        <v>3</v>
+        <v>39</v>
+      </c>
+      <c r="F12" s="14"/>
+      <c r="G12" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="11">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>23</v>
@@ -1100,7 +1116,7 @@
         <v>24</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>20</v>
@@ -1111,7 +1127,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>23</v>
@@ -1123,7 +1139,7 @@
         <v>24</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>20</v>
@@ -1134,7 +1150,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>23</v>
@@ -1146,7 +1162,7 @@
         <v>24</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>20</v>
@@ -1157,21 +1173,21 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="12" t="s">
         <v>24</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="G16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" t="s">
         <v>20</v>
       </c>
       <c r="H16" s="1">
@@ -1180,7 +1196,7 @@
     </row>
     <row r="17" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>23</v>
@@ -1192,9 +1208,9 @@
         <v>24</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" s="15"/>
+        <v>37</v>
+      </c>
+      <c r="F17" s="14"/>
       <c r="G17" s="9" t="s">
         <v>20</v>
       </c>
@@ -1204,7 +1220,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>23</v>
@@ -1216,66 +1232,65 @@
         <v>24</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>20</v>
       </c>
       <c r="H18" s="11">
+        <v>1</v>
+      </c>
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="1">
         <v>2</v>
       </c>
-      <c r="I18" s="5"/>
-    </row>
-    <row r="19" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="15"/>
-      <c r="G19" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" s="11">
+    </row>
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H20" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>65</v>
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>62</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>23</v>
@@ -1289,17 +1304,16 @@
       <c r="E21" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="15"/>
-      <c r="G21" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H21" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>65</v>
+      <c r="G21" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>60</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>23</v>
@@ -1311,42 +1325,42 @@
         <v>24</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F22" s="15"/>
-      <c r="G22" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H22" s="11">
+        <v>38</v>
+      </c>
+      <c r="G22" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="8" t="s">
+    <row r="23" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="12" t="s">
         <v>24</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H23" s="1">
-        <v>3</v>
+        <v>42</v>
+      </c>
+      <c r="F23" s="14"/>
+      <c r="G23" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23" s="11">
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>23</v>
@@ -1358,66 +1372,65 @@
         <v>24</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F24" s="15"/>
+        <v>33</v>
+      </c>
+      <c r="F24" s="14"/>
       <c r="G24" s="9" t="s">
         <v>20</v>
       </c>
       <c r="H24" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>24</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F25" s="15"/>
-      <c r="G25" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H25" s="11">
+        <v>34</v>
+      </c>
+      <c r="G25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H25" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="G26" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G26" s="6" t="s">
         <v>20</v>
       </c>
       <c r="H26" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>64</v>
+    <row r="27" spans="1:9" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>61</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>23</v>
@@ -1431,16 +1444,17 @@
       <c r="E27" s="13" t="s">
         <v>41</v>
       </c>
+      <c r="F27" s="14"/>
       <c r="G27" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H27" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
-        <v>64</v>
+      <c r="H27" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>62</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>23</v>
@@ -1451,19 +1465,20 @@
       <c r="D28" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E28" s="13" t="s">
-        <v>41</v>
-      </c>
+      <c r="E28" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F28" s="14"/>
       <c r="G28" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H28" s="1">
+      <c r="H28" s="11">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>23</v>
@@ -1474,19 +1489,19 @@
       <c r="D29" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E29" s="13" t="s">
-        <v>40</v>
+      <c r="E29" s="10" t="s">
+        <v>38</v>
       </c>
       <c r="G29" s="9" t="s">
         <v>20</v>
       </c>
       <c r="H29" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>67</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="B30" s="10" t="s">
         <v>23</v>
@@ -1497,20 +1512,19 @@
       <c r="D30" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E30" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="F30" s="15"/>
+      <c r="E30" s="10" t="s">
+        <v>33</v>
+      </c>
       <c r="G30" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H30" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
-        <v>67</v>
+      <c r="H30" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="B31" s="10" t="s">
         <v>23</v>
@@ -1521,21 +1535,34 @@
       <c r="D31" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E31" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="F31" s="15"/>
+      <c r="E31" s="10" t="s">
+        <v>35</v>
+      </c>
       <c r="G31" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H31" s="11">
+      <c r="H31" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
+    <row r="32" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E32" s="10"/>
+      <c r="F32" s="14"/>
+      <c r="H32" s="11"/>
+    </row>
+    <row r="33" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E33" s="10"/>
+      <c r="F33" s="14"/>
+      <c r="H33" s="11"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
     </row>
   </sheetData>
+  <sortState ref="A14:H18">
+    <sortCondition ref="H14:H18"/>
+    <sortCondition descending="1" ref="A14:A18"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
ssy19,ssy20,gsl2008 English Questionnaires added
- ssy19 ins1 + ssy20 ins1: Questionnaire_en, VariableQuestionnaire_en and QuestionFlow_en
- gsl2008 ins1-ins3: Questionnaire_en
</commit_message>
<xml_diff>
--- a/data/instruments/instruments.xlsx
+++ b/data/instruments/instruments.xlsx
@@ -11,12 +11,12 @@
     <sheet name="attachments" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="145621" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="81">
   <si>
     <t>title.de</t>
   </si>
@@ -247,6 +247,18 @@
   </si>
   <si>
     <t>subtitle.en</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>gsl2008_W1_Questionnaire_en.pdf</t>
+  </si>
+  <si>
+    <t>gsl2008_W2_Questionnaire_en.pdf</t>
+  </si>
+  <si>
+    <t>gsl2008_W3_Questionnaire_en.pdf</t>
   </si>
 </sst>
 </file>
@@ -787,10 +799,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,24 +864,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
+    <row r="3" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
+        <v>55</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>77</v>
       </c>
       <c r="G3" s="2">
         <v>1</v>
@@ -877,19 +889,19 @@
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>66</v>
+        <v>51</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>56</v>
       </c>
       <c r="F4" t="s">
         <v>19</v>
@@ -898,44 +910,44 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>45</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D6" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E6" s="14" t="s">
         <v>55</v>
-      </c>
-      <c r="F5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>56</v>
       </c>
       <c r="F6" t="s">
         <v>19</v>
@@ -944,90 +956,90 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
+    <row r="7" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="F7" t="s">
-        <v>19</v>
+        <v>50</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>77</v>
       </c>
       <c r="G7" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F8" t="s">
         <v>19</v>
       </c>
       <c r="G8" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>56</v>
+        <v>52</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="F9" t="s">
         <v>19</v>
       </c>
       <c r="G9" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>66</v>
+        <v>50</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>55</v>
       </c>
       <c r="F10" t="s">
         <v>19</v>
@@ -1036,79 +1048,87 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="11" t="s">
+      <c r="B14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="11" t="s">
         <v>38</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>29</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>19</v>
@@ -1117,192 +1137,192 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="7" t="s">
+    <row r="15" spans="1:8" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="1">
+        <v>37</v>
+      </c>
+      <c r="E15" s="12"/>
+      <c r="F15" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="6" t="s">
         <v>19</v>
       </c>
       <c r="G16" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="9" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G17" s="10">
+        <v>29</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="12"/>
+      <c r="F20" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="9" t="s">
+      <c r="B21" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" s="10">
+      <c r="F21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="10">
         <v>1</v>
       </c>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="11" t="s">
+      <c r="B22" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="F19" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G19" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G20" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>60</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F21" t="s">
-        <v>19</v>
-      </c>
-      <c r="G21" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="F22" s="6" t="s">
         <v>19</v>
       </c>
       <c r="G22" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" s="12"/>
-      <c r="F23" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G23" s="10">
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
-        <v>28</v>
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>60</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>22</v>
@@ -1311,28 +1331,27 @@
         <v>21</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G24" s="10">
+        <v>37</v>
+      </c>
+      <c r="F24" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>21</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F25" t="s">
         <v>19</v>
@@ -1341,29 +1360,30 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G26" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="12"/>
+      <c r="F26" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>22</v>
@@ -1371,110 +1391,171 @@
       <c r="C27" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="11" t="s">
-        <v>39</v>
+      <c r="D27" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="E27" s="12"/>
       <c r="F27" s="8" t="s">
         <v>19</v>
       </c>
       <c r="G27" s="10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C28" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" t="s">
         <v>21</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E28" s="12"/>
-      <c r="F28" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G28" s="10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="F28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F29" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F29" s="6" t="s">
         <v>19</v>
       </c>
       <c r="G29" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+    <row r="30" spans="1:8" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" s="12"/>
+      <c r="F30" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E31" s="12"/>
+      <c r="F31" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G31" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D30" s="9" t="s">
+      <c r="B33" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F30" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G30" s="1">
+      <c r="F33" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D31" s="9" t="s">
+      <c r="B34" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F31" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G31" s="1">
+      <c r="F34" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D32" s="9"/>
-      <c r="E32" s="12"/>
-      <c r="G32" s="10"/>
-    </row>
-    <row r="33" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D33" s="9"/>
-      <c r="E33" s="12"/>
-      <c r="G33" s="10"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
+    <row r="35" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D35" s="9"/>
+      <c r="E35" s="12"/>
+      <c r="G35" s="10"/>
+    </row>
+    <row r="36" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D36" s="9"/>
+      <c r="E36" s="12"/>
+      <c r="G36" s="10"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
     </row>
   </sheetData>
   <sortState ref="A14:H18">

</xml_diff>